<commit_message>
fix template and logic for administrational hours
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE223CE-CCDF-4046-80D3-1258E7A25A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>week of year</t>
   </si>
@@ -32,31 +33,19 @@
   </si>
   <si>
     <t>invoiced</t>
-  </si>
-  <si>
-    <t>21-11-2024</t>
-  </si>
-  <si>
-    <t>INVOICE #001</t>
-  </si>
-  <si>
-    <t>22-11-2024</t>
-  </si>
-  <si>
-    <t>23-11-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -414,21 +403,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="A2:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,66 +437,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>191</v>
-      </c>
-      <c r="D2">
-        <v>7.64</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>205</v>
-      </c>
-      <c r="D3">
-        <v>8.2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>47</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>225</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add more constants and fix template and logic for administrational hours
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE223CE-CCDF-4046-80D3-1258E7A25A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maher Gaming PC\Desktop\MTNA\invoicing-postnl-main\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>week of year</t>
   </si>
@@ -33,17 +37,83 @@
   </si>
   <si>
     <t>invoiced</t>
+  </si>
+  <si>
+    <t>02-12-2024</t>
+  </si>
+  <si>
+    <t>INVOICE #040</t>
+  </si>
+  <si>
+    <t>03-12-2024</t>
+  </si>
+  <si>
+    <t>04-12-2024</t>
+  </si>
+  <si>
+    <t>05-12-2024</t>
+  </si>
+  <si>
+    <t>06-12-2024</t>
+  </si>
+  <si>
+    <t>09-12-2024</t>
+  </si>
+  <si>
+    <t>10-12-2024</t>
+  </si>
+  <si>
+    <t>11-12-2024</t>
+  </si>
+  <si>
+    <t>12-12-2024</t>
+  </si>
+  <si>
+    <t>13-12-2024</t>
+  </si>
+  <si>
+    <t>14-12-2024</t>
+  </si>
+  <si>
+    <t>16-12-2024</t>
+  </si>
+  <si>
+    <t>17-12-2024</t>
+  </si>
+  <si>
+    <t>18-12-2024</t>
+  </si>
+  <si>
+    <t>19-12-2024</t>
+  </si>
+  <si>
+    <t>20-12-2024</t>
+  </si>
+  <si>
+    <t>21-12-2024</t>
+  </si>
+  <si>
+    <t>23-12-2024</t>
+  </si>
+  <si>
+    <t>24-12-2024</t>
+  </si>
+  <si>
+    <t>27-12-2024</t>
+  </si>
+  <si>
+    <t>28-12-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -57,13 +127,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -76,14 +140,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -92,10 +148,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -264,6 +320,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -290,24 +347,25 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -368,56 +426,32 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:G4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.832031" defaultRowHeight="16" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.16406" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="16.28516" customWidth="1"/>
+    <col min="5" max="5" width="11.83203" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="16" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,10 +471,340 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="10.16406" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="16.28516" customWidth="1"/>
+    <col min="5" max="5" width="11.83203" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16" customHeight="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" ht="16" customHeight="1">
+      <c r="A2">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>219</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" ht="16" customHeight="1">
+      <c r="A3">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>260</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" ht="16" customHeight="1">
+      <c r="A4">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>273</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" ht="16" customHeight="1">
+      <c r="A5">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>261</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" ht="16" customHeight="1">
+      <c r="A6">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>230</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>189</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" ht="16" customHeight="1">
+      <c r="A8">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>242</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>197</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>235</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" ht="16" customHeight="1">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>232</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" ht="16" customHeight="1">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>191</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" ht="16" customHeight="1">
+      <c r="A13">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>176</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" ht="16" customHeight="1">
+      <c r="A14">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>252</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" ht="16" customHeight="1">
+      <c r="A15">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>244</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" ht="16" customHeight="1">
+      <c r="A16">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>217</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" ht="16" customHeight="1">
+      <c r="A17">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>224</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" ht="16" customHeight="1">
+      <c r="A18">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>219</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" ht="16" customHeight="1">
+      <c r="A19">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>185</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" ht="16" customHeight="1">
+      <c r="A20">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>243</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" ht="16" customHeight="1">
+      <c r="A21">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>228</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" ht="16" customHeight="1">
+      <c r="A22">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>198</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix invoice number match regex
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maher Gaming PC\Desktop\MTNA\invoicing-postnl-main\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B634C50-95BE-9C4A-8C46-BEF0D2E0A5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>week of year</t>
   </si>
@@ -108,12 +105,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -127,7 +124,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -140,6 +143,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -148,10 +159,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -431,27 +442,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.832031" defaultRowHeight="16" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.16406" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="16.28516" customWidth="1"/>
-    <col min="5" max="5" width="11.83203" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16" customHeight="1">
+    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,26 +486,26 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.16406" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="16.28516" customWidth="1"/>
-    <col min="5" max="5" width="11.83203" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16" customHeight="1">
+    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="16" customHeight="1">
+    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>49</v>
       </c>
@@ -525,7 +539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" ht="16" customHeight="1">
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>49</v>
       </c>
@@ -539,7 +553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" ht="16" customHeight="1">
+    <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>49</v>
       </c>
@@ -553,7 +567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="16" customHeight="1">
+    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>49</v>
       </c>
@@ -567,7 +581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" ht="16" customHeight="1">
+    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>49</v>
       </c>
@@ -581,7 +595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="16" customHeight="1">
+    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>50</v>
       </c>
@@ -595,7 +609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" ht="16" customHeight="1">
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>50</v>
       </c>
@@ -609,7 +623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" ht="16" customHeight="1">
+    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>50</v>
       </c>
@@ -623,7 +637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" ht="16" customHeight="1">
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>50</v>
       </c>
@@ -637,7 +651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" ht="16" customHeight="1">
+    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>50</v>
       </c>
@@ -651,7 +665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" ht="16" customHeight="1">
+    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>50</v>
       </c>
@@ -665,7 +679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" ht="16" customHeight="1">
+    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>51</v>
       </c>
@@ -679,7 +693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" ht="16" customHeight="1">
+    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>51</v>
       </c>
@@ -693,7 +707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" ht="16" customHeight="1">
+    <row r="15" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>51</v>
       </c>
@@ -707,7 +721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" ht="16" customHeight="1">
+    <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>51</v>
       </c>
@@ -721,7 +735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" ht="16" customHeight="1">
+    <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>51</v>
       </c>
@@ -735,7 +749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" ht="16" customHeight="1">
+    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>51</v>
       </c>
@@ -749,7 +763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" ht="16" customHeight="1">
+    <row r="19" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>52</v>
       </c>
@@ -763,7 +777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" ht="16" customHeight="1">
+    <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>52</v>
       </c>
@@ -777,7 +791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" ht="16" customHeight="1">
+    <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>52</v>
       </c>
@@ -791,7 +805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" ht="16" customHeight="1">
+    <row r="22" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>52</v>
       </c>
@@ -806,5 +820,6 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>